<commit_message>
REALLY should've committed periodically
</commit_message>
<xml_diff>
--- a/Inventory.xlsx
+++ b/Inventory.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="172">
   <si>
     <t>Description</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Reference Field Detector diode</t>
   </si>
   <si>
-    <t>Type K Thermocouple Thermometer</t>
-  </si>
-  <si>
     <t>XAE080647</t>
   </si>
   <si>
@@ -506,13 +503,46 @@
   </si>
   <si>
     <t>part of 2241-3</t>
+  </si>
+  <si>
+    <t>60019</t>
+  </si>
+  <si>
+    <t>Micro Diamond single crystal diamond detector</t>
+  </si>
+  <si>
+    <t>123537</t>
+  </si>
+  <si>
+    <t>Lollipop Thermometer</t>
+  </si>
+  <si>
+    <t>Digisense</t>
+  </si>
+  <si>
+    <t>Traceable</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>200420520</t>
+  </si>
+  <si>
+    <t>Type K Thermometer</t>
+  </si>
+  <si>
+    <t>Thermocouple Thermometer</t>
+  </si>
+  <si>
+    <t>Digital Electronic Thermocouple Thermometer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Arial"/>
@@ -557,6 +587,12 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -785,7 +821,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -851,18 +887,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -934,6 +958,22 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1981,8 +2021,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Inventory" displayName="Inventory" ref="A7:O62" totalsRowShown="0" dataDxfId="15">
-  <autoFilter ref="A7:O62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Inventory" displayName="Inventory" ref="A7:O64" totalsRowShown="0" dataDxfId="15">
+  <autoFilter ref="A7:O64"/>
   <tableColumns count="15">
     <tableColumn id="14" name="Type" dataDxfId="14"/>
     <tableColumn id="10" name="Manufacturer" dataDxfId="13"/>
@@ -2311,10 +2351,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB62"/>
+  <dimension ref="A1:AB64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2338,60 +2378,60 @@
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" t="s">
         <v>134</v>
       </c>
-      <c r="H7" t="s">
-        <v>135</v>
-      </c>
       <c r="I7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J7" t="s">
         <v>2</v>
@@ -2400,16 +2440,16 @@
         <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N7" t="s">
         <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -2427,22 +2467,22 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="12">
         <v>2905</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G8" s="13" t="b">
         <v>0</v>
@@ -2474,22 +2514,22 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="12">
         <v>3704</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="13" t="b">
         <v>0</v>
@@ -2508,7 +2548,7 @@
       <c r="L9" s="15"/>
       <c r="M9" s="13"/>
       <c r="N9" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O9" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
@@ -2517,22 +2557,22 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" s="12">
         <v>619</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G10" s="13" t="b">
         <v>0</v>
@@ -2564,22 +2604,22 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>16</v>
+        <v>163</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="G11" s="13" t="b">
         <v>0</v>
@@ -2591,11 +2631,11 @@
         <v>2</v>
       </c>
       <c r="J11" s="15">
-        <v>44314</v>
+        <v>44068</v>
       </c>
       <c r="K11" s="3">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v>45044.5</v>
+        <v>44798.5</v>
       </c>
       <c r="L11" s="13" t="b">
         <v>0</v>
@@ -2603,32 +2643,30 @@
       <c r="M11" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="N11" s="16" t="s">
-        <v>121</v>
-      </c>
+      <c r="N11" s="11"/>
       <c r="O11" s="3">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v>45044.5</v>
+        <v>44798.5</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12" s="13" t="b">
         <v>0</v>
@@ -2640,44 +2678,44 @@
         <v>2</v>
       </c>
       <c r="J12" s="15">
-        <v>43906</v>
+        <v>44314</v>
       </c>
       <c r="K12" s="3">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v>44636.5</v>
+        <v>45044.5</v>
       </c>
       <c r="L12" s="13" t="b">
         <v>0</v>
       </c>
       <c r="M12" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O12" s="3" t="str">
-        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v/>
+        <v>120</v>
+      </c>
+      <c r="O12" s="3">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v>45044.5</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" s="13" t="b">
         <v>0</v>
@@ -2685,60 +2723,64 @@
       <c r="H13" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="3" t="str">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v/>
-      </c>
-      <c r="L13" s="15"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="3" t="str">
-        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v/>
+      <c r="I13" s="14">
+        <v>2</v>
+      </c>
+      <c r="J13" s="15">
+        <v>44686</v>
+      </c>
+      <c r="K13" s="3">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v>45416.5</v>
+      </c>
+      <c r="L13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="O13" s="3">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v>45416.5</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="G14" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="14">
-        <v>2</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>138</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="3" t="str">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
         <v/>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="13"/>
-      <c r="N14" s="16" t="s">
-        <v>19</v>
-      </c>
+      <c r="N14" s="11"/>
       <c r="O14" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -2746,65 +2788,65 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="11"/>
+        <v>93</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="E15" s="12" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="G15" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H15" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" s="14">
         <v>2</v>
       </c>
-      <c r="J15" s="15">
-        <v>44327</v>
-      </c>
-      <c r="K15" s="3">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v>45057.5</v>
-      </c>
-      <c r="L15" s="15" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" s="11"/>
-      <c r="O15" s="3">
-        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v>45057.5</v>
+      <c r="J15" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="K15" s="3" t="str">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v/>
+      </c>
+      <c r="L15" s="15"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="3" t="str">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="G16" s="13" t="b">
         <v>0</v>
@@ -2816,11 +2858,11 @@
         <v>2</v>
       </c>
       <c r="J16" s="15">
-        <v>44569</v>
+        <v>44327</v>
       </c>
       <c r="K16" s="3">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v>45299.5</v>
+        <v>45057.5</v>
       </c>
       <c r="L16" s="15" t="b">
         <v>0</v>
@@ -2831,27 +2873,25 @@
       <c r="N16" s="11"/>
       <c r="O16" s="3">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v>45299.5</v>
+        <v>45057.5</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="12">
-        <v>91697</v>
+        <v>12</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="G17" s="13" t="b">
         <v>0</v>
@@ -2859,38 +2899,46 @@
       <c r="H17" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="3" t="str">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v/>
-      </c>
-      <c r="L17" s="15"/>
-      <c r="M17" s="13"/>
+      <c r="I17" s="14">
+        <v>2</v>
+      </c>
+      <c r="J17" s="15">
+        <v>44569</v>
+      </c>
+      <c r="K17" s="3">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v>45299.5</v>
+      </c>
+      <c r="L17" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="13" t="b">
+        <v>0</v>
+      </c>
       <c r="N17" s="11"/>
-      <c r="O17" s="3" t="str">
-        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v/>
+      <c r="O17" s="3">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v>45299.5</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="E18" s="12">
-        <v>3829</v>
+        <v>91697</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G18" s="13" t="b">
         <v>0</v>
@@ -2898,185 +2946,177 @@
       <c r="H18" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="14">
-        <v>1</v>
-      </c>
-      <c r="J18" s="15">
-        <v>44283</v>
-      </c>
-      <c r="K18" s="3">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v>44648.25</v>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="3" t="str">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v/>
       </c>
       <c r="L18" s="15"/>
-      <c r="M18" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="M18" s="13"/>
       <c r="N18" s="11"/>
       <c r="O18" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="12">
-        <v>3949</v>
+        <v>3829</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G19" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="14">
         <v>1</v>
       </c>
-      <c r="J19" s="23">
-        <v>44446</v>
+      <c r="J19" s="15">
+        <v>44686</v>
       </c>
       <c r="K19" s="3">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v>44811.25</v>
+        <v>45051.25</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="N19" s="24" t="s">
+      <c r="N19" s="11"/>
+      <c r="O19" s="3">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v>45051.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="12">
+        <v>3949</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="42">
+        <v>1</v>
+      </c>
+      <c r="J20" s="43">
+        <v>44446</v>
+      </c>
+      <c r="K20" s="3">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v>44811.25</v>
+      </c>
+      <c r="L20" s="15"/>
+      <c r="M20" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="O20" s="3">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v>44811.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="25">
+        <v>248122</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="27">
+        <v>1</v>
+      </c>
+      <c r="J21" s="28">
+        <v>44573</v>
+      </c>
+      <c r="K21" s="29">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v>44938.25</v>
+      </c>
+      <c r="L21" s="28"/>
+      <c r="M21" s="26" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="O19" s="3">
-        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v>44811.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="27" t="s">
+      <c r="O21" s="3">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v>44938.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="28">
-        <v>248122</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="30">
-        <v>1</v>
-      </c>
-      <c r="J20" s="31">
-        <v>44573</v>
-      </c>
-      <c r="K20" s="32">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v>44938.25</v>
-      </c>
-      <c r="L20" s="31"/>
-      <c r="M20" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="N20" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="O20" s="3">
-        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v>44938.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E22" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="21">
-        <v>1</v>
-      </c>
-      <c r="J21" s="17">
-        <v>44573</v>
-      </c>
-      <c r="K21" s="10">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v>44938.25</v>
-      </c>
-      <c r="L21" s="17"/>
-      <c r="M21" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="N21" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="O21" s="3">
-        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v>44938.25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>79</v>
+      <c r="F22" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="G22" s="18" t="b">
         <v>0</v>
@@ -3098,118 +3138,126 @@
       <c r="M22" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="N22" s="35" t="s">
-        <v>161</v>
+      <c r="N22" s="32" t="s">
+        <v>160</v>
       </c>
       <c r="O22" s="3">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v>44938.25</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="37" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="21">
+        <v>1</v>
+      </c>
+      <c r="J23" s="17">
+        <v>44573</v>
+      </c>
+      <c r="K23" s="10">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v>44938.25</v>
+      </c>
+      <c r="L23" s="17"/>
+      <c r="M23" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="O23" s="3">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v>44938.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="E24" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="39" t="b">
+      <c r="F24" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I24" s="37">
         <v>1</v>
       </c>
-      <c r="J23" s="41">
+      <c r="J24" s="38">
         <v>44573</v>
       </c>
-      <c r="K23" s="42">
+      <c r="K24" s="39">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
         <v>44938.25</v>
       </c>
-      <c r="L23" s="41"/>
-      <c r="M23" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="N23" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="O23" s="3">
+      <c r="L24" s="38"/>
+      <c r="M24" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="O24" s="3">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v>44938.25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="3" t="str">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v/>
-      </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="3" t="str">
-        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
-        <v/>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>105</v>
-      </c>
       <c r="D25" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G25" s="13" t="b">
         <v>0</v>
@@ -3233,20 +3281,22 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="11"/>
+        <v>104</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="E26" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G26" s="13" t="b">
         <v>0</v>
@@ -3270,22 +3320,20 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>36</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="D27" s="11"/>
       <c r="E27" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G27" s="13" t="b">
         <v>0</v>
@@ -3309,20 +3357,22 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>43</v>
+        <v>106</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="12"/>
+        <v>35</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>110</v>
+      </c>
       <c r="F28" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G28" s="13" t="b">
         <v>0</v>
@@ -3330,14 +3380,11 @@
       <c r="H28" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="I28" s="14">
-        <v>2</v>
-      </c>
-      <c r="J28" s="15">
-        <v>43496</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>138</v>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="3" t="str">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v/>
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="13"/>
@@ -3349,18 +3396,18 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="11"/>
+        <v>41</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D29" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="12">
-        <v>95788</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E29" s="12"/>
       <c r="F29" s="12" t="s">
         <v>76</v>
       </c>
@@ -3370,11 +3417,14 @@
       <c r="H29" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="I29" s="14"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="3" t="str">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v/>
+      <c r="I29" s="14">
+        <v>2</v>
+      </c>
+      <c r="J29" s="15">
+        <v>43496</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="L29" s="15"/>
       <c r="M29" s="13"/>
@@ -3386,20 +3436,20 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E30" s="12">
-        <v>1342006</v>
+        <v>95788</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G30" s="13" t="b">
         <v>0</v>
@@ -3423,20 +3473,20 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31" s="12">
-        <v>106634</v>
+        <v>1342006</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G31" s="13" t="b">
         <v>0</v>
@@ -3460,30 +3510,28 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E32" s="12">
-        <v>3704</v>
+        <v>106634</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="G32" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H32" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="14">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I32" s="14"/>
       <c r="J32" s="15"/>
       <c r="K32" s="3" t="str">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
@@ -3491,9 +3539,7 @@
       </c>
       <c r="L32" s="15"/>
       <c r="M32" s="13"/>
-      <c r="N32" s="16" t="s">
-        <v>19</v>
-      </c>
+      <c r="N32" s="11"/>
       <c r="O32" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -3501,22 +3547,20 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>114</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C33" s="11"/>
       <c r="D33" s="11" t="s">
-        <v>116</v>
+        <v>23</v>
       </c>
       <c r="E33" s="12">
-        <v>108070</v>
+        <v>3704</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="G33" s="13" t="b">
         <v>0</v>
@@ -3524,7 +3568,9 @@
       <c r="H33" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="14"/>
+      <c r="I33" s="14">
+        <v>2</v>
+      </c>
       <c r="J33" s="15"/>
       <c r="K33" s="3" t="str">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
@@ -3532,7 +3578,9 @@
       </c>
       <c r="L33" s="15"/>
       <c r="M33" s="13"/>
-      <c r="N33" s="11"/>
+      <c r="N33" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="O33" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -3540,28 +3588,28 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="E34" s="12">
-        <v>108079</v>
+        <v>108070</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G34" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H34" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="14"/>
       <c r="J34" s="15"/>
@@ -3579,10 +3627,10 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>114</v>
@@ -3591,16 +3639,16 @@
         <v>116</v>
       </c>
       <c r="E35" s="12">
-        <v>108069</v>
+        <v>108079</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G35" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H35" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="14"/>
       <c r="J35" s="15"/>
@@ -3618,28 +3666,28 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>117</v>
-      </c>
       <c r="E36" s="12">
-        <v>108070</v>
+        <v>108069</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G36" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H36" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" s="14"/>
       <c r="J36" s="15"/>
@@ -3657,24 +3705,28 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>114</v>
+      </c>
       <c r="D37" s="11" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="E37" s="12">
-        <v>340705</v>
+        <v>108070</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G37" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H37" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="14"/>
       <c r="J37" s="15"/>
@@ -3684,9 +3736,7 @@
       </c>
       <c r="L37" s="15"/>
       <c r="M37" s="13"/>
-      <c r="N37" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="N37" s="11"/>
       <c r="O37" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -3694,16 +3744,18 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="12"/>
+        <v>37</v>
+      </c>
+      <c r="E38" s="12">
+        <v>340705</v>
+      </c>
       <c r="F38" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G38" s="13" t="b">
         <v>0</v>
@@ -3719,7 +3771,9 @@
       </c>
       <c r="L38" s="15"/>
       <c r="M38" s="13"/>
-      <c r="N38" s="11"/>
+      <c r="N38" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="O38" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -3727,16 +3781,16 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" s="12"/>
       <c r="F39" s="12" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G39" s="13" t="b">
         <v>0</v>
@@ -3760,28 +3814,24 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" s="12">
-        <v>440883</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E40" s="12"/>
       <c r="F40" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G40" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H40" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="14" t="s">
-        <v>133</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I40" s="14"/>
       <c r="J40" s="15"/>
       <c r="K40" s="3" t="str">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
@@ -3797,25 +3847,31 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>169</v>
+      </c>
       <c r="D41" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="12"/>
+        <v>170</v>
+      </c>
+      <c r="E41" s="12">
+        <v>440883</v>
+      </c>
       <c r="F41" s="12" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="G41" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H41" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J41" s="15"/>
       <c r="K41" s="3" t="str">
@@ -3832,31 +3888,34 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>164</v>
+      </c>
       <c r="D42" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>168</v>
+      </c>
       <c r="F42" s="12" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="G42" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H42" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" s="14">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="J42" s="15"/>
-      <c r="K42" s="3" t="str">
-        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
-        <v/>
-      </c>
+      <c r="K42" s="3"/>
       <c r="L42" s="15"/>
       <c r="M42" s="13"/>
       <c r="N42" s="11"/>
@@ -3865,26 +3924,32 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
+        <v>68</v>
+      </c>
+      <c r="B43" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="D43" s="11" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="12" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="G43" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H43" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>132</v>
+      </c>
       <c r="J43" s="15"/>
       <c r="K43" s="3" t="str">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
@@ -3892,9 +3957,7 @@
       </c>
       <c r="L43" s="15"/>
       <c r="M43" s="13"/>
-      <c r="N43" s="16" t="s">
-        <v>19</v>
-      </c>
+      <c r="N43" s="11"/>
       <c r="O43" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -3902,12 +3965,12 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E44" s="12"/>
       <c r="F44" s="12" t="s">
@@ -3919,8 +3982,8 @@
       <c r="H44" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="I44" s="14" t="s">
-        <v>133</v>
+      <c r="I44" s="14">
+        <v>4</v>
       </c>
       <c r="J44" s="15"/>
       <c r="K44" s="3" t="str">
@@ -3937,20 +4000,14 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>124</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="12">
-        <v>330025</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E45" s="12"/>
       <c r="F45" s="12" t="s">
         <v>79</v>
       </c>
@@ -3968,7 +4025,9 @@
       </c>
       <c r="L45" s="15"/>
       <c r="M45" s="13"/>
-      <c r="N45" s="11"/>
+      <c r="N45" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="O45" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -3976,22 +4035,16 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>126</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
       <c r="D46" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E46" s="12">
-        <v>5283306</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E46" s="12"/>
       <c r="F46" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G46" s="13" t="b">
         <v>0</v>
@@ -3999,7 +4052,9 @@
       <c r="H46" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="I46" s="14"/>
+      <c r="I46" s="14" t="s">
+        <v>132</v>
+      </c>
       <c r="J46" s="15"/>
       <c r="K46" s="3" t="str">
         <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
@@ -4018,19 +4073,19 @@
         <v>71</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E47" s="12">
-        <v>5498918</v>
+        <v>330025</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G47" s="13" t="b">
         <v>0</v>
@@ -4054,20 +4109,22 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="12"/>
+        <v>22</v>
+      </c>
+      <c r="E48" s="12">
+        <v>5283306</v>
+      </c>
       <c r="F48" s="12" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="G48" s="13" t="b">
         <v>0</v>
@@ -4091,16 +4148,22 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="D49" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="12"/>
+        <v>126</v>
+      </c>
+      <c r="E49" s="12">
+        <v>5498918</v>
+      </c>
       <c r="F49" s="12" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="G49" s="13" t="b">
         <v>0</v>
@@ -4124,18 +4187,20 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="C50" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="E50" s="12"/>
       <c r="F50" s="12" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="G50" s="13" t="b">
         <v>0</v>
@@ -4159,22 +4224,22 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
       <c r="D51" s="11" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="12" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="G51" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H51" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="14"/>
       <c r="J51" s="15"/>
@@ -4192,22 +4257,24 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
+      <c r="C52" s="11" t="s">
+        <v>128</v>
+      </c>
       <c r="D52" s="11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G52" s="13" t="b">
         <v>0</v>
       </c>
       <c r="H52" s="13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="14"/>
       <c r="J52" s="15"/>
@@ -4225,16 +4292,16 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
       <c r="D53" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G53" s="13" t="b">
         <v>0</v>
@@ -4258,16 +4325,16 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
       <c r="D54" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E54" s="12"/>
       <c r="F54" s="12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="G54" s="13" t="b">
         <v>0</v>
@@ -4291,16 +4358,16 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="11"/>
       <c r="D55" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="12" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="G55" s="13" t="b">
         <v>0</v>
@@ -4324,7 +4391,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -4333,7 +4400,7 @@
       </c>
       <c r="E56" s="12"/>
       <c r="F56" s="12" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="G56" s="13" t="b">
         <v>0</v>
@@ -4357,20 +4424,16 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>118</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="11" t="s">
-        <v>142</v>
+        <v>53</v>
       </c>
       <c r="E57" s="12"/>
       <c r="F57" s="12" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="G57" s="13" t="b">
         <v>0</v>
@@ -4394,33 +4457,32 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>145</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I58" s="21"/>
-      <c r="J58" s="17"/>
-      <c r="K58" s="10"/>
-      <c r="L58" s="17"/>
-      <c r="M58" s="18"/>
-      <c r="N58" s="19"/>
+        <v>55</v>
+      </c>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G58" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" s="14"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="3" t="str">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v/>
+      </c>
+      <c r="L58" s="15"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="11"/>
       <c r="O58" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -4428,33 +4490,36 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>144</v>
+        <v>11</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="E59" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="F59" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I59" s="21"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="10"/>
-      <c r="L59" s="17"/>
-      <c r="M59" s="18"/>
-      <c r="N59" s="19"/>
+        <v>141</v>
+      </c>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G59" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="14"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="3" t="str">
+        <f>IF(AND(ISNUMBER(Inventory[TG-40 req for cal]),ISNUMBER(Inventory[Date last cal])),Inventory[Date last cal]+Inventory[TG-40 req for cal]*365.25,"")</f>
+        <v/>
+      </c>
+      <c r="L59" s="15"/>
+      <c r="M59" s="13"/>
+      <c r="N59" s="11"/>
       <c r="O59" s="3" t="str">
         <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
         <v/>
@@ -4462,21 +4527,23 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="E60" s="13" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F60" s="19"/>
+        <v>145</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="G60" s="18"/>
       <c r="H60" s="18" t="b">
         <v>1</v>
@@ -4494,22 +4561,22 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B61" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="C61" s="11" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="G61" s="18"/>
       <c r="H61" s="18" t="b">
@@ -4528,21 +4595,25 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B62" s="11" t="s">
-        <v>159</v>
-      </c>
       <c r="C62" s="11" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E62" s="11"/>
+        <v>153</v>
+      </c>
+      <c r="E62" s="13" t="e">
+        <v>#N/A</v>
+      </c>
       <c r="F62" s="19"/>
       <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
+      <c r="H62" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="I62" s="21"/>
       <c r="J62" s="17"/>
       <c r="K62" s="10"/>
@@ -4554,46 +4625,102 @@
         <v/>
       </c>
     </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" s="21"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="18"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="3" t="str">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E64" s="11"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="18"/>
+      <c r="N64" s="19"/>
+      <c r="O64" s="3" t="str">
+        <f ca="1">IF(AND(Inventory[[Preparing for cal]:[Preparing for cal]]=FALSE,Inventory[[Out for cal]:[Out for cal]]=FALSE,NOT(ISERROR(DATE(YEAR(Inventory[[Cal due date]:[Cal due date]]), MONTH(Inventory[[Cal due date]:[Cal due date]]), DAY(Inventory[[Cal due date]:[Cal due date]])))),Inventory[[Cal due date]:[Cal due date]]&gt;=TODAY()),Inventory[[Cal due date]:[Cal due date]],"")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="A8:N62">
-    <cfRule type="expression" dxfId="19" priority="10">
+  <conditionalFormatting sqref="A8:N64">
+    <cfRule type="expression" dxfId="19" priority="18">
       <formula>AND($L8=TRUE,$K8&gt;=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$M8=TRUE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="12">
+    <cfRule type="expression" dxfId="17" priority="20">
       <formula>AND($K8&lt;TODAY(),NOT(ISBLANK($M8)),$M8=FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="13">
+    <cfRule type="expression" dxfId="16" priority="21">
       <formula>$K8=MIN($O:$O)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Input" error="Must be a value from the dropdown list" sqref="A8:A62">
-      <formula1>"Annual QA equipment,Barometer,Daily/monthly QA equipment,Electrometer,Film equipment,In-vivo dosimeter,Ion chamber,Linac,Room monitor,Scanning detector,Software,Survey meter,Thermometer"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Input" error="Must be a value from the dropdown list" sqref="B8:B62">
-      <formula1>"Accuray,Elekta,Fluke,IBA,Ludlum,MIM,PTW,RaySearch,Scanditronix,Standard Imaging,Sun Nuclear,Varian,Victoreen,Vidar"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Input" error="Must be a value from the dropdown list" sqref="F8:F62">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Input" error="Must be a value from the dropdown list" sqref="F8:F64">
       <formula1>"Block room,E1 closet,E1 console,E1 vault,E2 closet,E2 console,E2 vault,Elekta console,Elekta vault,Hot lab,Physics cabinet,Physics mid room,Physics office,Tomo closet,Tomo console,Tomo vault"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Input" error="Must be TRUE or FALSE" sqref="G8:H62">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Input" error="Must be TRUE or FALSE" sqref="G8:H64">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I62">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I64">
       <formula1>IF(ISERROR(VALUE($I8)),LOWER($I8)="initial use",AND(VALUE($I8)=INT($I8),$I8&gt;0))</formula1>
     </dataValidation>
-    <dataValidation type="custom" showErrorMessage="1" errorTitle="Invalid Input" error="If there is no due date, must be empty_x000a_If preparing for cal, must be FALSE_x000a_Otherwise, must be TRUE or FALSE" sqref="M8:M62">
+    <dataValidation type="custom" showErrorMessage="1" errorTitle="Invalid Input" error="If there is no due date, must be empty_x000a_If preparing for cal, must be FALSE_x000a_Otherwise, must be TRUE or FALSE" sqref="M8:M64">
       <formula1>IF(ISERROR(DATE(YEAR($K8),MONTH($K8),DAY($K8))),ISBLANK($L8),IF($L8=TRUE,$M8=FALSE,OR($M8=TRUE,$M8=FALSE)))</formula1>
     </dataValidation>
-    <dataValidation type="custom" showErrorMessage="1" errorTitle="Invalid Input" error="If no due date, must be empty_x000a_Otherwise, must be TRUE or FALSE" sqref="L8:L62">
-      <formula1>IF(ISERROR(DATE(YEAR($K8),MONTH($K8),DAY($K8))),ISBLANK($L8),OR($L8=TRUE,$L8=FALSE))</formula1>
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Input" error="Must be a past date or &quot;not req'd&quot; (case insensitive)" sqref="J8:J64">
+      <formula1>OR(LOWER($J8)="not req'd", AND(ISNUMBER($J8), $J8&lt;=TODAY()))</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Input" error="Must be a past date or &quot;not req'd&quot; (case insensitive)" sqref="J8:J62">
-      <formula1>OR(LOWER($J8)="not req'd", AND(ISNUMBER($J8), $J8&lt;=TODAY()))</formula1>
+    <dataValidation type="custom" showErrorMessage="1" errorTitle="Invalid Input" error="If no due date, must be empty_x000a_Otherwise, must be TRUE or FALSE" sqref="L1:L1048576">
+      <formula1>IF(ISERROR(DATE(YEAR($K1),MONTH($K1),DAY($K1))),ISBLANK($L1),OR($L1=TRUE,$L1=FALSE))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="1" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>